<commit_message>
done with col names map
</commit_message>
<xml_diff>
--- a/data_cleaning/datasets_raw/MS Form - POST Connection - COMMERCIAL & INSTITUTION Connection Impact Survey.xlsx
+++ b/data_cleaning/datasets_raw/MS Form - POST Connection - COMMERCIAL & INSTITUTION Connection Impact Survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\aorsot\Renewvia\survey_impact_analysis\data_cleaning\datasets_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A46A9F-EAF8-494F-9863-CBEBFD149320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BE1357-18E1-4ED4-86A1-12FE1DB5093B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7596,13 +7596,13 @@
     <t>For businesses or shop owners only: Since connection to Renewvia minigrid, have you seen any change in your weekly or monthly earnings?</t>
   </si>
   <si>
-    <t>If you have closed operations, please explain@ why:</t>
-  </si>
-  <si>
-    <t>If you answered yes to above, please explain@:</t>
-  </si>
-  <si>
-    <t>If you answered yes to the question above, please explain@:</t>
+    <t>If you have closed operations, please explain* why:</t>
+  </si>
+  <si>
+    <t>If you answered yes to above, please explain*:</t>
+  </si>
+  <si>
+    <t>If you answered yes to the question above, please explain*:</t>
   </si>
 </sst>
 </file>
@@ -7798,7 +7798,7 @@
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Please select your business type" dataDxfId="25"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="What is the name of your business/school/clinic/religious institution?" dataDxfId="24"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Is this business, clinic, school still in operation?" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="If you have closed operations, please explain@ why:" dataDxfId="22"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="If you have closed operations, please explain* why:" dataDxfId="22"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Do you have any other sources of electricity other than Renewvia Minigrid?" dataDxfId="21"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Since connection to Renewvia minigrid, what appliances have you added to your business operations?" dataDxfId="20"/>
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="If you selected &quot;other electronic device&quot; above, please list what it is:" dataDxfId="19"/>
@@ -7808,9 +7808,9 @@
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="If you answered &quot;yes, they have increased&quot; above, by how many hours have they increased?" dataDxfId="15"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Since connection to Renewvia minigrid, has your access to clean drinking water changed at all?" dataDxfId="14"/>
     <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Have you added any new products or services since connection to Renewvia minigrid?" dataDxfId="13"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="If you answered yes to above, please explain@:" dataDxfId="12"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="If you answered yes to above, please explain*:" dataDxfId="12"/>
     <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Since connection to Renewvia mingrid, have you had any change in number of workers/employees at your place of work?" dataDxfId="11"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="If you answered yes to the question above, please explain@:" dataDxfId="10"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="If you answered yes to the question above, please explain*:" dataDxfId="10"/>
     <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="If you answered yes to adding new workers, how many new employees are female?" dataDxfId="9"/>
     <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="For businesses or shop owners only: Since connection to Renewvia minigrid, have you seen any change in your weekly or monthly earnings?" dataDxfId="8"/>
     <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="What services are you able to offer/sell/provide due to connection to Renewvia minigrid that you weren't able to offer prior to connection?" dataDxfId="7"/>
@@ -8125,8 +8125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK395"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47699,15 +47699,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038073657E5DB2D47AAD91621692220EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="afb3daf45c20648a38b84a160d60719d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="996edba2-ec33-4a2e-8368-78d9e900b9f2" xmlns:ns3="5210dd66-3e32-4fad-90ef-2e158a04e990" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b6a9de8e624e0e032ad798c972482c2" ns2:_="" ns3:_="">
     <xsd:import namespace="996edba2-ec33-4a2e-8368-78d9e900b9f2"/>
@@ -47930,6 +47921,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{927AA0EB-35C6-41B2-8EBA-E658C6B34E37}">
   <ds:schemaRefs>
@@ -47942,14 +47942,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D12A8A5-769E-41F1-B474-AC1310E723F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A65EE60-DB6C-4697-B61B-90A21A3592FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -47966,4 +47958,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D12A8A5-769E-41F1-B474-AC1310E723F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>